<commit_message>
update results of mf
</commit_message>
<xml_diff>
--- a/docs/matlab/ml-100k.xlsx
+++ b/docs/matlab/ml-100k.xlsx
@@ -134,7 +134,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -179,8 +179,16 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -193,6 +201,11 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -203,10 +216,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -223,9 +239,13 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="好" xfId="1" builtinId="26"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -7466,8 +7486,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AM89"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -7520,7 +7540,7 @@
       <c r="AM1" s="3"/>
     </row>
     <row r="2" spans="1:39" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="8" t="s">
         <v>27</v>
       </c>
       <c r="B2" s="4" t="s">

</xml_diff>

<commit_message>
update mf vs f
</commit_message>
<xml_diff>
--- a/docs/matlab/ml-100k.xlsx
+++ b/docs/matlab/ml-100k.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="33">
   <si>
     <t>N</t>
   </si>
@@ -129,6 +129,10 @@
     <t>u3.base/u3.test</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>f</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -222,7 +226,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -240,6 +244,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -7484,10 +7491,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AM89"/>
+  <dimension ref="A1:AM145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A75" sqref="A75:G118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -14416,148 +14423,1076 @@
         <v>7.8461087111265898E-2</v>
       </c>
     </row>
+    <row r="75" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A75" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B75" s="3"/>
+      <c r="C75" s="3"/>
+      <c r="D75" s="3"/>
+      <c r="E75" s="3"/>
+      <c r="F75" s="3"/>
+      <c r="G75" s="3"/>
+    </row>
+    <row r="76" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A76" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B76" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C76" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D76" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E76" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F76" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G76" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="77" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A77" s="5">
+        <v>10</v>
+      </c>
+      <c r="B77" s="6">
+        <v>1</v>
+      </c>
+      <c r="C77" s="6">
+        <v>0.25945945945945897</v>
+      </c>
+      <c r="D77" s="6">
+        <v>1.2E-2</v>
+      </c>
+      <c r="E77" s="6">
+        <v>7.5151515151515205E-2</v>
+      </c>
+      <c r="F77" s="6">
+        <v>6.0360356568085596</v>
+      </c>
+      <c r="G77" s="6">
+        <v>0.52980132450331097</v>
+      </c>
+    </row>
     <row r="78" spans="1:39" x14ac:dyDescent="0.2">
-      <c r="A78" t="s">
+      <c r="A78" s="5"/>
+      <c r="B78" s="6">
+        <v>5</v>
+      </c>
+      <c r="C78" s="6">
+        <v>0.223783783783784</v>
+      </c>
+      <c r="D78" s="6">
+        <v>5.1749999999999997E-2</v>
+      </c>
+      <c r="E78" s="6">
+        <v>0.16727272727272699</v>
+      </c>
+      <c r="F78" s="6">
+        <v>5.96736028596069</v>
+      </c>
+      <c r="G78" s="6">
+        <v>0.36838116261957299</v>
+      </c>
+    </row>
+    <row r="79" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A79" s="5"/>
+      <c r="B79" s="6">
+        <v>10</v>
+      </c>
+      <c r="C79" s="6">
+        <v>0.200756756756757</v>
+      </c>
+      <c r="D79" s="6">
+        <v>9.2850000000000002E-2</v>
+      </c>
+      <c r="E79" s="6">
+        <v>0.237575757575758</v>
+      </c>
+      <c r="F79" s="6">
+        <v>5.9201359522169001</v>
+      </c>
+      <c r="G79" s="6">
+        <v>0.29825475664879603</v>
+      </c>
+    </row>
+    <row r="80" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A80" s="5"/>
+      <c r="B80" s="6">
+        <v>15</v>
+      </c>
+      <c r="C80" s="6">
+        <v>0.182702702702703</v>
+      </c>
+      <c r="D80" s="6">
+        <v>0.12675</v>
+      </c>
+      <c r="E80" s="6">
+        <v>0.30363636363636398</v>
+      </c>
+      <c r="F80" s="6">
+        <v>5.8891776205772297</v>
+      </c>
+      <c r="G80" s="6">
+        <v>0.25871257146091597</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A81" s="5"/>
+      <c r="B81" s="6">
+        <v>20</v>
+      </c>
+      <c r="C81" s="6">
+        <v>0.16874831035415</v>
+      </c>
+      <c r="D81" s="6">
+        <v>0.15604999999999999</v>
+      </c>
+      <c r="E81" s="6">
+        <v>0.35939393939393899</v>
+      </c>
+      <c r="F81" s="6">
+        <v>5.8652417709897602</v>
+      </c>
+      <c r="G81" s="6">
+        <v>0.229332219248682</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A82" s="5"/>
+      <c r="B82" s="6">
+        <v>25</v>
+      </c>
+      <c r="C82" s="6">
+        <v>0.15737775854608399</v>
+      </c>
+      <c r="D82" s="6">
+        <v>0.18185000000000001</v>
+      </c>
+      <c r="E82" s="6">
+        <v>0.40727272727272701</v>
+      </c>
+      <c r="F82" s="6">
+        <v>5.8459204718958597</v>
+      </c>
+      <c r="G82" s="6">
+        <v>0.20711129555048299</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A83" s="5"/>
+      <c r="B83" s="6">
+        <v>30</v>
+      </c>
+      <c r="C83" s="6">
+        <v>0.147339945897205</v>
+      </c>
+      <c r="D83" s="6">
+        <v>0.20424999999999999</v>
+      </c>
+      <c r="E83" s="6">
+        <v>0.44606060606060599</v>
+      </c>
+      <c r="F83" s="6">
+        <v>5.8307522530225402</v>
+      </c>
+      <c r="G83" s="6">
+        <v>0.18844955035914501</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A84" s="5">
+        <v>20</v>
+      </c>
+      <c r="B84" s="6">
+        <v>1</v>
+      </c>
+      <c r="C84" s="6">
+        <v>0.27891891891891901</v>
+      </c>
+      <c r="D84" s="6">
+        <v>1.29E-2</v>
+      </c>
+      <c r="E84" s="6">
+        <v>7.7575757575757603E-2</v>
+      </c>
+      <c r="F84" s="6">
+        <v>6.0365060542084699</v>
+      </c>
+      <c r="G84" s="6">
+        <v>0.56953642384105996</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A85" s="5"/>
+      <c r="B85" s="6">
+        <v>5</v>
+      </c>
+      <c r="C85" s="6">
+        <v>0.23200000000000001</v>
+      </c>
+      <c r="D85" s="6">
+        <v>5.3650000000000003E-2</v>
+      </c>
+      <c r="E85" s="6">
+        <v>0.17272727272727301</v>
+      </c>
+      <c r="F85" s="6">
+        <v>5.9616744758709697</v>
+      </c>
+      <c r="G85" s="6">
+        <v>0.39142016188373802</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A86" s="5"/>
+      <c r="B86" s="6">
+        <v>10</v>
+      </c>
+      <c r="C86" s="6">
+        <v>0.20735135135135099</v>
+      </c>
+      <c r="D86" s="6">
+        <v>9.5899999999999999E-2</v>
+      </c>
+      <c r="E86" s="6">
+        <v>0.25090909090909103</v>
+      </c>
+      <c r="F86" s="6">
+        <v>5.9163665420518496</v>
+      </c>
+      <c r="G86" s="6">
+        <v>0.31625030659798897</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A87" s="5"/>
+      <c r="B87" s="6">
+        <v>15</v>
+      </c>
+      <c r="C87" s="6">
+        <v>0.18731531531531501</v>
+      </c>
+      <c r="D87" s="6">
+        <v>0.12995000000000001</v>
+      </c>
+      <c r="E87" s="6">
+        <v>0.31454545454545502</v>
+      </c>
+      <c r="F87" s="6">
+        <v>5.8854716023620899</v>
+      </c>
+      <c r="G87" s="6">
+        <v>0.27234336957295002</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A88" s="5"/>
+      <c r="B88" s="6">
+        <v>20</v>
+      </c>
+      <c r="C88" s="6">
+        <v>0.17437145174371499</v>
+      </c>
+      <c r="D88" s="6">
+        <v>0.16125</v>
+      </c>
+      <c r="E88" s="6">
+        <v>0.36666666666666697</v>
+      </c>
+      <c r="F88" s="6">
+        <v>5.86171874388672</v>
+      </c>
+      <c r="G88" s="6">
+        <v>0.24320480779793599</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A89" s="5"/>
+      <c r="B89" s="6">
+        <v>25</v>
+      </c>
+      <c r="C89" s="6">
+        <v>0.16356555603634801</v>
+      </c>
+      <c r="D89" s="6">
+        <v>0.189</v>
+      </c>
+      <c r="E89" s="6">
+        <v>0.40606060606060601</v>
+      </c>
+      <c r="F89" s="6">
+        <v>5.8426071397515296</v>
+      </c>
+      <c r="G89" s="6">
+        <v>0.220827535743328</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A90" s="5"/>
+      <c r="B90" s="6">
+        <v>30</v>
+      </c>
+      <c r="C90" s="6">
+        <v>0.15336339044184</v>
+      </c>
+      <c r="D90" s="6">
+        <v>0.21260000000000001</v>
+      </c>
+      <c r="E90" s="6">
+        <v>0.441212121212121</v>
+      </c>
+      <c r="F90" s="6">
+        <v>5.8264053894908896</v>
+      </c>
+      <c r="G90" s="6">
+        <v>0.20154096345748199</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A91" s="5">
+        <v>50</v>
+      </c>
+      <c r="B91" s="6">
+        <v>1</v>
+      </c>
+      <c r="C91" s="6">
+        <v>0.29297297297297298</v>
+      </c>
+      <c r="D91" s="6">
+        <v>1.355E-2</v>
+      </c>
+      <c r="E91" s="6">
+        <v>8.3636363636363606E-2</v>
+      </c>
+      <c r="F91" s="6">
+        <v>6.0290572136268201</v>
+      </c>
+      <c r="G91" s="6">
+        <v>0.59823399558498902</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A92" s="5"/>
+      <c r="B92" s="6">
+        <v>5</v>
+      </c>
+      <c r="C92" s="6">
+        <v>0.23913513513513501</v>
+      </c>
+      <c r="D92" s="6">
+        <v>5.5300000000000002E-2</v>
+      </c>
+      <c r="E92" s="6">
+        <v>0.18484848484848501</v>
+      </c>
+      <c r="F92" s="6">
+        <v>5.9604646054545896</v>
+      </c>
+      <c r="G92" s="6">
+        <v>0.41003679175864599</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A93" s="5"/>
+      <c r="B93" s="6">
+        <v>10</v>
+      </c>
+      <c r="C93" s="6">
+        <v>0.21264864864864899</v>
+      </c>
+      <c r="D93" s="6">
+        <v>9.8350000000000007E-2</v>
+      </c>
+      <c r="E93" s="6">
+        <v>0.25878787878787901</v>
+      </c>
+      <c r="F93" s="6">
+        <v>5.9112123312284401</v>
+      </c>
+      <c r="G93" s="6">
+        <v>0.33012736956445599</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A94" s="5"/>
+      <c r="B94" s="6">
+        <v>15</v>
+      </c>
+      <c r="C94" s="6">
+        <v>0.19776576576576599</v>
+      </c>
+      <c r="D94" s="6">
+        <v>0.13719999999999999</v>
+      </c>
+      <c r="E94" s="6">
+        <v>0.31636363636363601</v>
+      </c>
+      <c r="F94" s="6">
+        <v>5.8795181788009598</v>
+      </c>
+      <c r="G94" s="6">
+        <v>0.29016315219405697</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A95" s="5"/>
+      <c r="B95" s="6">
+        <v>20</v>
+      </c>
+      <c r="C95" s="6">
+        <v>0.17945390646120599</v>
+      </c>
+      <c r="D95" s="6">
+        <v>0.16594999999999999</v>
+      </c>
+      <c r="E95" s="6">
+        <v>0.36606060606060598</v>
+      </c>
+      <c r="F95" s="6">
+        <v>5.8554702128999896</v>
+      </c>
+      <c r="G95" s="6">
+        <v>0.25503162727761902</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A96" s="5"/>
+      <c r="B96" s="6">
+        <v>25</v>
+      </c>
+      <c r="C96" s="6">
+        <v>0.16564257897014301</v>
+      </c>
+      <c r="D96" s="6">
+        <v>0.19139999999999999</v>
+      </c>
+      <c r="E96" s="6">
+        <v>0.413333333333333</v>
+      </c>
+      <c r="F96" s="6">
+        <v>5.8362266116977803</v>
+      </c>
+      <c r="G96" s="6">
+        <v>0.228394212100478</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A97" s="5"/>
+      <c r="B97" s="6">
+        <v>30</v>
+      </c>
+      <c r="C97" s="6">
+        <v>0.15603246167718701</v>
+      </c>
+      <c r="D97" s="6">
+        <v>0.21629999999999999</v>
+      </c>
+      <c r="E97" s="6">
+        <v>0.44909090909090899</v>
+      </c>
+      <c r="F97" s="6">
+        <v>5.8203452026367204</v>
+      </c>
+      <c r="G97" s="6">
+        <v>0.208302014151728</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A98" s="5">
+        <v>100</v>
+      </c>
+      <c r="B98" s="6">
+        <v>1</v>
+      </c>
+      <c r="C98" s="6">
+        <v>0.30810810810810801</v>
+      </c>
+      <c r="D98" s="6">
+        <v>1.4250000000000001E-2</v>
+      </c>
+      <c r="E98" s="6">
+        <v>8.24242424242424E-2</v>
+      </c>
+      <c r="F98" s="6">
+        <v>6.0126417993544097</v>
+      </c>
+      <c r="G98" s="6">
+        <v>0.629139072847682</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A99" s="5"/>
+      <c r="B99" s="6">
+        <v>5</v>
+      </c>
+      <c r="C99" s="6">
+        <v>0.24929729729729699</v>
+      </c>
+      <c r="D99" s="6">
+        <v>5.765E-2</v>
+      </c>
+      <c r="E99" s="6">
+        <v>0.18242424242424199</v>
+      </c>
+      <c r="F99" s="6">
+        <v>5.9509425705263297</v>
+      </c>
+      <c r="G99" s="6">
+        <v>0.43581309786607803</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A100" s="5"/>
+      <c r="B100" s="6">
+        <v>10</v>
+      </c>
+      <c r="C100" s="6">
+        <v>0.22010810810810799</v>
+      </c>
+      <c r="D100" s="6">
+        <v>0.1018</v>
+      </c>
+      <c r="E100" s="6">
+        <v>0.25878787878787901</v>
+      </c>
+      <c r="F100" s="6">
+        <v>5.9070913792940303</v>
+      </c>
+      <c r="G100" s="6">
+        <v>0.350040032937384</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A101" s="5"/>
+      <c r="B101" s="6">
+        <v>15</v>
+      </c>
+      <c r="C101" s="6">
+        <v>0.197981981981982</v>
+      </c>
+      <c r="D101" s="6">
+        <v>0.13735</v>
+      </c>
+      <c r="E101" s="6">
+        <v>0.32666666666666699</v>
+      </c>
+      <c r="F101" s="6">
+        <v>5.8765455808045797</v>
+      </c>
+      <c r="G101" s="6">
+        <v>0.29882914199691302</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A102" s="5"/>
+      <c r="B102" s="6">
+        <v>20</v>
+      </c>
+      <c r="C102" s="6">
+        <v>0.181995133819951</v>
+      </c>
+      <c r="D102" s="6">
+        <v>0.16830000000000001</v>
+      </c>
+      <c r="E102" s="6">
+        <v>0.37636363636363601</v>
+      </c>
+      <c r="F102" s="6">
+        <v>5.8530949452426002</v>
+      </c>
+      <c r="G102" s="6">
+        <v>0.26366189971376203</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A103" s="5"/>
+      <c r="B103" s="6">
+        <v>25</v>
+      </c>
+      <c r="C103" s="6">
+        <v>0.169839896148853</v>
+      </c>
+      <c r="D103" s="6">
+        <v>0.19625000000000001</v>
+      </c>
+      <c r="E103" s="6">
+        <v>0.41818181818181799</v>
+      </c>
+      <c r="F103" s="6">
+        <v>5.8338003057053403</v>
+      </c>
+      <c r="G103" s="6">
+        <v>0.237881051126688</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A104" s="5"/>
+      <c r="B104" s="6">
+        <v>30</v>
+      </c>
+      <c r="C104" s="6">
+        <v>0.16014427412082999</v>
+      </c>
+      <c r="D104" s="6">
+        <v>0.222</v>
+      </c>
+      <c r="E104" s="6">
+        <v>0.45696969696969703</v>
+      </c>
+      <c r="F104" s="6">
+        <v>5.8180361193366403</v>
+      </c>
+      <c r="G104" s="6">
+        <v>0.218211821564815</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A105" s="5">
+        <v>200</v>
+      </c>
+      <c r="B105" s="6">
+        <v>1</v>
+      </c>
+      <c r="C105" s="6">
+        <v>0.32</v>
+      </c>
+      <c r="D105" s="6">
+        <v>1.4800000000000001E-2</v>
+      </c>
+      <c r="E105" s="6">
+        <v>8.3636363636363606E-2</v>
+      </c>
+      <c r="F105" s="6">
+        <v>6.02390411185345</v>
+      </c>
+      <c r="G105" s="6">
+        <v>0.653421633554084</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A106" s="5"/>
+      <c r="B106" s="6">
+        <v>5</v>
+      </c>
+      <c r="C106" s="6">
+        <v>0.248648648648649</v>
+      </c>
+      <c r="D106" s="6">
+        <v>5.7500000000000002E-2</v>
+      </c>
+      <c r="E106" s="6">
+        <v>0.18060606060606099</v>
+      </c>
+      <c r="F106" s="6">
+        <v>5.9598503411820696</v>
+      </c>
+      <c r="G106" s="6">
+        <v>0.434716703458425</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A107" s="5"/>
+      <c r="B107" s="6">
+        <v>10</v>
+      </c>
+      <c r="C107" s="6">
+        <v>0.21945945945945899</v>
+      </c>
+      <c r="D107" s="6">
+        <v>0.10150000000000001</v>
+      </c>
+      <c r="E107" s="6">
+        <v>0.25636363636363602</v>
+      </c>
+      <c r="F107" s="6">
+        <v>5.9140223866744996</v>
+      </c>
+      <c r="G107" s="6">
+        <v>0.34791031570832898</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A108" s="5"/>
+      <c r="B108" s="6">
+        <v>15</v>
+      </c>
+      <c r="C108" s="6">
+        <v>0.19870270270270299</v>
+      </c>
+      <c r="D108" s="6">
+        <v>0.13785</v>
+      </c>
+      <c r="E108" s="6">
+        <v>0.31515151515151502</v>
+      </c>
+      <c r="F108" s="6">
+        <v>5.8825179020970904</v>
+      </c>
+      <c r="G108" s="6">
+        <v>0.298643788963877</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A109" s="5"/>
+      <c r="B109" s="6">
+        <v>20</v>
+      </c>
+      <c r="C109" s="6">
+        <v>0.183400919167343</v>
+      </c>
+      <c r="D109" s="6">
+        <v>0.1696</v>
+      </c>
+      <c r="E109" s="6">
+        <v>0.37212121212121202</v>
+      </c>
+      <c r="F109" s="6">
+        <v>5.85755082309129</v>
+      </c>
+      <c r="G109" s="6">
+        <v>0.26514381534902598</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A110" s="5"/>
+      <c r="B110" s="6">
+        <v>25</v>
+      </c>
+      <c r="C110" s="6">
+        <v>0.17144093466032001</v>
+      </c>
+      <c r="D110" s="6">
+        <v>0.1981</v>
+      </c>
+      <c r="E110" s="6">
+        <v>0.42060606060606098</v>
+      </c>
+      <c r="F110" s="6">
+        <v>5.8373364150560096</v>
+      </c>
+      <c r="G110" s="6">
+        <v>0.23996902776273901</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A111" s="5"/>
+      <c r="B111" s="6">
+        <v>30</v>
+      </c>
+      <c r="C111" s="6">
+        <v>0.16068530207394</v>
+      </c>
+      <c r="D111" s="6">
+        <v>0.22275</v>
+      </c>
+      <c r="E111" s="6">
+        <v>0.46</v>
+      </c>
+      <c r="F111" s="6">
+        <v>5.8209305558277302</v>
+      </c>
+      <c r="G111" s="6">
+        <v>0.218925360204444</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A112" s="5">
+        <v>500</v>
+      </c>
+      <c r="B112" s="6">
+        <v>1</v>
+      </c>
+      <c r="C112" s="6">
+        <v>0.302702702702703</v>
+      </c>
+      <c r="D112" s="6">
+        <v>1.4E-2</v>
+      </c>
+      <c r="E112" s="6">
+        <v>0.08</v>
+      </c>
+      <c r="F112" s="6">
+        <v>6.0390286091184704</v>
+      </c>
+      <c r="G112" s="6">
+        <v>0.61810154525386296</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A113" s="5"/>
+      <c r="B113" s="6">
+        <v>5</v>
+      </c>
+      <c r="C113" s="6">
+        <v>0.245837837837838</v>
+      </c>
+      <c r="D113" s="6">
+        <v>5.6849999999999998E-2</v>
+      </c>
+      <c r="E113" s="6">
+        <v>0.17151515151515201</v>
+      </c>
+      <c r="F113" s="6">
+        <v>5.9604217496928698</v>
+      </c>
+      <c r="G113" s="6">
+        <v>0.42637969094922701</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A114" s="5"/>
+      <c r="B114" s="6">
+        <v>10</v>
+      </c>
+      <c r="C114" s="6">
+        <v>0.22</v>
+      </c>
+      <c r="D114" s="6">
+        <v>0.10174999999999999</v>
+      </c>
+      <c r="E114" s="6">
+        <v>0.24727272727272701</v>
+      </c>
+      <c r="F114" s="6">
+        <v>5.9083041743702198</v>
+      </c>
+      <c r="G114" s="6">
+        <v>0.34765242300010502</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A115" s="5"/>
+      <c r="B115" s="6">
+        <v>15</v>
+      </c>
+      <c r="C115" s="6">
+        <v>0.197621621621622</v>
+      </c>
+      <c r="D115" s="6">
+        <v>0.1371</v>
+      </c>
+      <c r="E115" s="6">
+        <v>0.321212121212121</v>
+      </c>
+      <c r="F115" s="6">
+        <v>5.8748262308433503</v>
+      </c>
+      <c r="G115" s="6">
+        <v>0.29658545893645299</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A116" s="5"/>
+      <c r="B116" s="6">
+        <v>20</v>
+      </c>
+      <c r="C116" s="6">
+        <v>0.184103811841038</v>
+      </c>
+      <c r="D116" s="6">
+        <v>0.17025000000000001</v>
+      </c>
+      <c r="E116" s="6">
+        <v>0.37636363636363601</v>
+      </c>
+      <c r="F116" s="6">
+        <v>5.8508209144220604</v>
+      </c>
+      <c r="G116" s="6">
+        <v>0.26527213697949797</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A117" s="5"/>
+      <c r="B117" s="6">
+        <v>25</v>
+      </c>
+      <c r="C117" s="6">
+        <v>0.17070532237126801</v>
+      </c>
+      <c r="D117" s="6">
+        <v>0.19725000000000001</v>
+      </c>
+      <c r="E117" s="6">
+        <v>0.42181818181818198</v>
+      </c>
+      <c r="F117" s="6">
+        <v>5.8310296224060298</v>
+      </c>
+      <c r="G117" s="6">
+        <v>0.23805582077656101</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A118" s="5"/>
+      <c r="B118" s="6">
+        <v>30</v>
+      </c>
+      <c r="C118" s="6">
+        <v>0.160108205590622</v>
+      </c>
+      <c r="D118" s="6">
+        <v>0.22195000000000001</v>
+      </c>
+      <c r="E118" s="6">
+        <v>0.46181818181818202</v>
+      </c>
+      <c r="F118" s="6">
+        <v>5.8154975980783199</v>
+      </c>
+      <c r="G118" s="6">
+        <v>0.21694171128557299</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A134" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="79" spans="1:39" x14ac:dyDescent="0.2">
-      <c r="A79" s="2" t="s">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A135" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B79" s="2">
+      <c r="B135" s="2">
         <v>1</v>
       </c>
-      <c r="C79" s="2"/>
-      <c r="D79" s="2"/>
-      <c r="E79" s="2"/>
-      <c r="F79" s="2"/>
-    </row>
-    <row r="80" spans="1:39" x14ac:dyDescent="0.2">
-      <c r="A80" s="3" t="s">
+      <c r="C135" s="2"/>
+      <c r="D135" s="2"/>
+      <c r="E135" s="2"/>
+      <c r="F135" s="2"/>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A136" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B80" s="3"/>
-      <c r="C80" s="3"/>
-      <c r="D80" s="3"/>
-      <c r="E80" s="3"/>
-      <c r="F80" s="3"/>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A81" s="3" t="s">
+      <c r="B136" s="3"/>
+      <c r="C136" s="3"/>
+      <c r="D136" s="3"/>
+      <c r="E136" s="3"/>
+      <c r="F136" s="3"/>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A137" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B81" s="3">
+      <c r="B137" s="3">
         <v>160000</v>
       </c>
-      <c r="C81" s="3"/>
-      <c r="D81" s="3"/>
-      <c r="E81" s="3"/>
-      <c r="F81" s="3"/>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A82" s="3" t="s">
+      <c r="C137" s="3"/>
+      <c r="D137" s="3"/>
+      <c r="E137" s="3"/>
+      <c r="F137" s="3"/>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A138" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B82" s="3">
+      <c r="B138" s="3">
         <v>20000</v>
       </c>
-      <c r="C82" s="3"/>
-      <c r="D82" s="3"/>
-      <c r="E82" s="3"/>
-      <c r="F82" s="3"/>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A83" s="3" t="s">
+      <c r="C138" s="3"/>
+      <c r="D138" s="3"/>
+      <c r="E138" s="3"/>
+      <c r="F138" s="3"/>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A139" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B83" s="3">
+      <c r="B139" s="3">
         <v>943</v>
       </c>
-      <c r="C83" s="3" t="s">
+      <c r="C139" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D83" s="3">
+      <c r="D139" s="3">
         <v>1682</v>
       </c>
-      <c r="E83" s="3" t="s">
+      <c r="E139" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F83" s="3">
+      <c r="F139" s="3">
         <v>100</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A84" s="3" t="s">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A140" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B84" s="3">
+      <c r="B140" s="3">
         <v>100</v>
       </c>
-      <c r="C84" s="3"/>
-      <c r="D84" s="3"/>
-      <c r="E84" s="3"/>
-      <c r="F84" s="3"/>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A85" s="3" t="s">
+      <c r="C140" s="3"/>
+      <c r="D140" s="3"/>
+      <c r="E140" s="3"/>
+      <c r="F140" s="3"/>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A141" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B85" s="3">
+      <c r="B141" s="3">
         <v>0.02</v>
       </c>
-      <c r="C85" s="3"/>
-      <c r="D85" s="3"/>
-      <c r="E85" s="3"/>
-      <c r="F85" s="3"/>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A86" s="3" t="s">
+      <c r="C141" s="3"/>
+      <c r="D141" s="3"/>
+      <c r="E141" s="3"/>
+      <c r="F141" s="3"/>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A142" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B86" s="3">
+      <c r="B142" s="3">
         <v>0.01</v>
       </c>
-      <c r="C86" s="3"/>
-      <c r="D86" s="3"/>
-      <c r="E86" s="3"/>
-      <c r="F86" s="3"/>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A87" s="3" t="s">
+      <c r="C142" s="3"/>
+      <c r="D142" s="3"/>
+      <c r="E142" s="3"/>
+      <c r="F142" s="3"/>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A143" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B87" s="3">
+      <c r="B143" s="3">
         <v>0.9</v>
       </c>
-      <c r="C87" s="3"/>
-      <c r="D87" s="3"/>
-      <c r="E87" s="3"/>
-      <c r="F87" s="3"/>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A88" s="3" t="s">
+      <c r="C143" s="3"/>
+      <c r="D143" s="3"/>
+      <c r="E143" s="3"/>
+      <c r="F143" s="3"/>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A144" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B88" s="3">
+      <c r="B144" s="3">
         <v>1</v>
       </c>
-      <c r="C88" s="3"/>
-      <c r="D88" s="3"/>
-      <c r="E88" s="3"/>
-      <c r="F88" s="3"/>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A89" s="3" t="s">
+      <c r="C144" s="3"/>
+      <c r="D144" s="3"/>
+      <c r="E144" s="3"/>
+      <c r="F144" s="3"/>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A145" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B89" s="3">
+      <c r="B145" s="3">
         <v>5</v>
       </c>
-      <c r="C89" s="3"/>
-      <c r="D89" s="3"/>
-      <c r="E89" s="3"/>
-      <c r="F89" s="3"/>
+      <c r="C145" s="3"/>
+      <c r="D145" s="3"/>
+      <c r="E145" s="3"/>
+      <c r="F145" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>